<commit_message>
New topics are updated
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen S\IdeaProjects\java_tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0908846-2885-4DD6-9ADC-B995F2DEEDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7B26A0-0E8D-4735-B0D7-925D4A154D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{EAC3D683-8219-47E3-9D1A-5258474EDC66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="16" xr2:uid="{EAC3D683-8219-47E3-9D1A-5258474EDC66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,14 @@
     <sheet name="CharacterSequence" sheetId="7" r:id="rId7"/>
     <sheet name="Collections" sheetId="8" r:id="rId8"/>
     <sheet name="Methods" sheetId="9" r:id="rId9"/>
-    <sheet name="Access Specifiers" sheetId="10" r:id="rId10"/>
+    <sheet name="Oops" sheetId="11" r:id="rId10"/>
+    <sheet name="Constructor and Destructor" sheetId="12" r:id="rId11"/>
+    <sheet name="Polymorphism" sheetId="13" r:id="rId12"/>
+    <sheet name="Inheritance" sheetId="14" r:id="rId13"/>
+    <sheet name="Packages" sheetId="15" r:id="rId14"/>
+    <sheet name="Access Specifiers" sheetId="10" r:id="rId15"/>
+    <sheet name="Interface and abstract class" sheetId="16" r:id="rId16"/>
+    <sheet name="Exception Handling" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="341">
   <si>
     <t>Variables &amp; Datatype</t>
   </si>
@@ -720,13 +727,361 @@
   </si>
   <si>
     <t>to handle zero/multiple arguments</t>
+  </si>
+  <si>
+    <t>Class &amp; Object</t>
+  </si>
+  <si>
+    <t>Abstraction</t>
+  </si>
+  <si>
+    <t>Encapsulation</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>Classes &amp; Object</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Behaviors</t>
+  </si>
+  <si>
+    <t>Data Member</t>
+  </si>
+  <si>
+    <t>Member Methods</t>
+  </si>
+  <si>
+    <t>Static/Non-Static</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>Meeting1</t>
+  </si>
+  <si>
+    <t>Meeting2</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Syntax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classname </t>
+  </si>
+  <si>
+    <t>objectname</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new </t>
+  </si>
+  <si>
+    <t>classname();</t>
+  </si>
+  <si>
+    <t>Properties/(Instance/Object) Properties/Non Static</t>
+  </si>
+  <si>
+    <t>Class Properties/Static</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>We can access the data member/member method of the class, outside or main function with the help of Object</t>
+  </si>
+  <si>
+    <t>Rules regarding static</t>
+  </si>
+  <si>
+    <t>Static DataMember/Member Method can be accessed in both non Static/static member method</t>
+  </si>
+  <si>
+    <t>Non Static Data Member/Member Method can be accessed only in Non static member methods</t>
+  </si>
+  <si>
+    <t>We can access the data member/member method(static) of the class, outside or main function with the help of Class name/without the class name aswell</t>
+  </si>
+  <si>
+    <t>Why public static void main(String[] args){}</t>
+  </si>
+  <si>
+    <t>access modifier should be public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">static is used so that it can drirectly called/loaded in the memory </t>
+  </si>
+  <si>
+    <t>void because main methods does not return anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constructor name and class name should be same </t>
+  </si>
+  <si>
+    <t>Constructor is a special method which has parameters but no return type/return statement</t>
+  </si>
+  <si>
+    <t>Constructor method will be called when the object is created</t>
+  </si>
+  <si>
+    <t>Constructor is used to initialize object</t>
+  </si>
+  <si>
+    <t>It is not necessary for you to created constructor. Becase by default you will be a having constructor for the class and it called as "Default Constructor"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Constructor </t>
+  </si>
+  <si>
+    <t>We use constructor mostly to initialize the value for objects properties</t>
+  </si>
+  <si>
+    <t>Constructor cannot be a static</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of Constructor </t>
+  </si>
+  <si>
+    <t>Non-parameterized constructor</t>
+  </si>
+  <si>
+    <t>Parameterized constructor</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>keyword referes the current class object/instance</t>
+  </si>
+  <si>
+    <t>Destructor</t>
+  </si>
+  <si>
+    <t>used to release the memory occupied by the object</t>
+  </si>
+  <si>
+    <t>No need to write explicit. Because destrcutor will be called automatically at the end of your program</t>
+  </si>
+  <si>
+    <t>Garbage collection</t>
+  </si>
+  <si>
+    <t>finalize() -&gt; will be called to release all the memory occupied by the object</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Overloading</t>
+  </si>
+  <si>
+    <t>Overriding</t>
+  </si>
+  <si>
+    <t>Same name but different in their charateristics (no. or type of parameter)</t>
+  </si>
+  <si>
+    <t>Same name but same in their charateristics (no. or type of parameter)</t>
+  </si>
+  <si>
+    <t>Methods, Constructor</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Multilevel</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Hirerachy</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>no supported</t>
+  </si>
+  <si>
+    <t>Base Class</t>
+  </si>
+  <si>
+    <t>Derived Class</t>
+  </si>
+  <si>
+    <t>Parent Class</t>
+  </si>
+  <si>
+    <t>Child Class</t>
+  </si>
+  <si>
+    <t>inside any package, if I create 2 or more classes and If communicate within them how to do it.</t>
+  </si>
+  <si>
+    <t>in different package, if I create 2 or more classes and If communicate within them how to do it.</t>
+  </si>
+  <si>
+    <t>Super Class</t>
+  </si>
+  <si>
+    <t>Sub Class</t>
+  </si>
+  <si>
+    <t>Same Package</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Non sub class</t>
+  </si>
+  <si>
+    <t>Other Package</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Protected</t>
+  </si>
+  <si>
+    <t>Privated</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Cannot be accessed outside of the class</t>
+  </si>
+  <si>
+    <t>Abstract Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstract </t>
+  </si>
+  <si>
+    <t>Non Abstarct</t>
+  </si>
+  <si>
+    <t>You cannot created a object</t>
+  </si>
+  <si>
+    <t>a process of hiding the implementation details and showing the functionality</t>
+  </si>
+  <si>
+    <t>Abstract Method</t>
+  </si>
+  <si>
+    <t>is just declared not implemented in the Abstract class. But it has be implemented in the derieved class</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>abstract &amp; non abstract method</t>
+  </si>
+  <si>
+    <t>abstract method</t>
+  </si>
+  <si>
+    <t>multiple inheritance not supported</t>
+  </si>
+  <si>
+    <t>multiple inheritance is supported</t>
+  </si>
+  <si>
+    <t>extends</t>
+  </si>
+  <si>
+    <t>implements</t>
+  </si>
+  <si>
+    <t>it always a public/default specifier</t>
+  </si>
+  <si>
+    <t>private, protected, default, public non abstract methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public abstract method/ in interface all the abstracts methods are treated as public </t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>finally</t>
+  </si>
+  <si>
+    <t>throw</t>
+  </si>
+  <si>
+    <t>throws</t>
+  </si>
+  <si>
+    <t>for try you should have either catch or finally block</t>
+  </si>
+  <si>
+    <t>ArrayIndexOutOfBoundsException</t>
+  </si>
+  <si>
+    <t>InputMismatchException</t>
+  </si>
+  <si>
+    <t>Can I use multiple catch? Yes</t>
+  </si>
+  <si>
+    <t>throw any exception from code</t>
+  </si>
+  <si>
+    <t>ArithmeticException</t>
+  </si>
+  <si>
+    <t>5/0</t>
+  </si>
+  <si>
+    <t>final vs finally vs finalize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,8 +1089,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,8 +1116,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -757,11 +1137,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -769,6 +1201,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -780,6 +1223,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,285 +1620,285 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>44593</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>44594</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>44594</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>44600</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>44600</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>44602</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>44603</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>44604</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>44605</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>44606</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>44607</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>44608</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>44609</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>44610</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>44611</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>44612</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>44613</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>44614</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>44615</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>44616</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>44617</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>44618</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>44619</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>44620</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>44621</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>44622</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>44623</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>44624</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>44625</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>44626</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1457,47 +1910,785 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA6DD0D-71C4-49AB-84EB-5C01D19B9E73}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C58139-80D3-4314-9D2E-90721E081BCF}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="E9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="D15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="D16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32A535A-E448-4B9F-8B05-026F0B8C07E3}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="C19" activeCellId="1" sqref="B18 C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C17BD52-CC75-4C8C-A461-C953B6D306C5}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="61.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B579CC-8799-44AA-85B9-0F0527297252}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" t="s">
+        <v>297</v>
+      </c>
+      <c r="I3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H4" t="s">
+        <v>298</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+      <c r="J4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517C7D27-5B23-40F0-B31D-28D41964BE44}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA6DD0D-71C4-49AB-84EB-5C01D19B9E73}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="E5" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E6" s="19"/>
+      <c r="F6" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>204</v>
       </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="E8" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="E9" s="19"/>
+      <c r="F9" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A346AB56-8F3E-42CA-A1F8-76306D6EC5FF}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" customWidth="1"/>
+    <col min="7" max="7" width="70" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="F10" t="s">
+        <v>310</v>
+      </c>
+      <c r="G10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="F12" t="s">
+        <v>319</v>
+      </c>
+      <c r="G12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="F13" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="F14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="F15" t="s">
+        <v>326</v>
+      </c>
+      <c r="G15" t="s">
+        <v>327</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE71FBC-0F11-45D6-90F6-C4DACFA4A657}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="J4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="C7" s="20" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="C8" s="20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="C9" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1509,13 +2700,13 @@
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1523,7 +2714,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1531,7 +2722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1542,27 +2733,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1580,64 +2771,64 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="B2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -1645,7 +2836,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="C12" t="s">
         <v>44</v>
       </c>
@@ -1659,7 +2850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="C13" t="s">
         <v>45</v>
       </c>
@@ -1673,7 +2864,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="C14" t="s">
         <v>46</v>
       </c>
@@ -1684,65 +2875,65 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="C15" t="s">
         <v>47</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="15" t="s">
         <v>53</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="C16" t="s">
         <v>42</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="15"/>
       <c r="G16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="C17" t="s">
         <v>48</v>
       </c>
       <c r="D17">
         <v>8</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="15"/>
       <c r="G17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="C18" t="s">
         <v>43</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="45" customHeight="1">
       <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="D19">
         <v>8</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="16"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -1750,57 +2941,57 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="C22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="C23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="C24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="B26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="C27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="C28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="C29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="C30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="C31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>65</v>
       </c>
@@ -1808,7 +2999,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -1834,7 +3025,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -1844,7 +3035,7 @@
     <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1873,7 +3064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1887,7 +3078,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="F3" t="s">
         <v>90</v>
       </c>
@@ -1895,7 +3086,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1912,7 +3103,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="B5" t="s">
         <v>83</v>
       </c>
@@ -1923,7 +3114,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="B6" s="4" t="s">
         <v>84</v>
       </c>
@@ -1934,12 +3125,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="B7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="B8" t="s">
         <v>86</v>
       </c>
@@ -1956,7 +3147,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="28.8">
       <c r="E9" s="3" t="s">
         <v>109</v>
       </c>
@@ -1967,7 +3158,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>111</v>
       </c>
@@ -1978,7 +3169,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -1997,7 +3188,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" customWidth="1"/>
@@ -2005,7 +3196,7 @@
     <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2015,36 +3206,36 @@
       <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="12.6" customHeight="1">
       <c r="B3" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="F5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="G6" t="s">
         <v>121</v>
       </c>
@@ -2052,7 +3243,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="G7" t="s">
         <v>122</v>
       </c>
@@ -2060,7 +3251,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -2071,7 +3262,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -2095,13 +3286,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2109,37 +3300,37 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="C7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="C8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="C10" t="s">
         <v>132</v>
       </c>
@@ -2160,7 +3351,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
@@ -2170,7 +3361,7 @@
     <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2181,7 +3372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2201,7 +3392,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2231,17 +3422,17 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -2258,7 +3449,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -2272,7 +3463,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -2286,7 +3477,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -2297,12 +3488,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="E6" t="s">
         <v>173</v>
       </c>
@@ -2313,7 +3504,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>158</v>
       </c>
@@ -2321,7 +3512,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>149</v>
       </c>
@@ -2344,7 +3535,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -2370,7 +3561,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -2393,7 +3584,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -2416,7 +3607,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -2430,7 +3621,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -2447,12 +3638,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -2466,7 +3657,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -2480,7 +3671,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -2494,7 +3685,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
         <v>181</v>
       </c>
@@ -2511,7 +3702,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -2519,7 +3710,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>183</v>
       </c>
@@ -2527,7 +3718,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>191</v>
       </c>
@@ -2544,11 +3735,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3894CC6C-5D2A-406A-8AF1-9BDAFAA2BAE7}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
@@ -2556,12 +3747,12 @@
     <col min="5" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>192</v>
       </c>
@@ -2569,17 +3760,17 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="D4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="C5" t="s">
         <v>195</v>
       </c>
@@ -2593,7 +3784,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>206</v>
       </c>
@@ -2610,7 +3801,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>215</v>
       </c>
@@ -2624,7 +3815,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>216</v>
       </c>
@@ -2638,7 +3829,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="C11" t="s">
         <v>211</v>
       </c>
@@ -2646,7 +3837,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>210</v>
       </c>
@@ -2657,7 +3848,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>221</v>
       </c>
@@ -2671,7 +3862,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>224</v>
       </c>

</xml_diff>